<commit_message>
add genx example system
</commit_message>
<xml_diff>
--- a/NREL_PVPro/load_profile_San Diego_CA-3.xlsx
+++ b/NREL_PVPro/load_profile_San Diego_CA-3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Future_Power_Grid/Project2/NREL_PVPro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E6A1913-81F5-6842-A835-6F52B709A4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{501EE0EE-7E5E-4449-AB2B-A9DA494AC61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="2220" yWindow="1600" windowWidth="27240" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="load_profile_San Diego_CA-3" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculate net load profile
</commit_message>
<xml_diff>
--- a/NREL_PVPro/load_profile_San Diego_CA-3.xlsx
+++ b/NREL_PVPro/load_profile_San Diego_CA-3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Future_Power_Grid/Project2/NREL_PVPro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{501EE0EE-7E5E-4449-AB2B-A9DA494AC61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5F5A4C-8F82-4945-B606-75A3F2340F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="1600" windowWidth="27240" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="2220" yWindow="1600" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="load_profile_San Diego_CA-3" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -9864,8 +9864,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Weekday_EV_Load" displayName="Weekday_EV_Load" ref="A1:H97" totalsRowShown="0">
-  <autoFilter ref="A1:H97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Weekday_EV_Load" displayName="Weekday_EV_Load" ref="A1:H97" totalsRowShown="0">
+  <autoFilter ref="A1:H97" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -9876,14 +9876,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Time" dataDxfId="3"/>
-    <tableColumn id="2" name="home_l1"/>
-    <tableColumn id="3" name="home_l2"/>
-    <tableColumn id="4" name="work_l1"/>
-    <tableColumn id="5" name="work_l2"/>
-    <tableColumn id="6" name="public_l2"/>
-    <tableColumn id="7" name="public_l3"/>
-    <tableColumn id="8" name="total" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Time" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="home_l1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="home_l2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="work_l1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="work_l2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="public_l2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="public_l3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="total" dataDxfId="2">
       <calculatedColumnFormula>SUM(Weekday_EV_Load[[#This Row],[home_l1]:[public_l3]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9892,8 +9892,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Weekend_EV_Load" displayName="Weekend_EV_Load" ref="J1:Q97" totalsRowShown="0">
-  <autoFilter ref="J1:Q97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Weekend_EV_Load" displayName="Weekend_EV_Load" ref="J1:Q97" totalsRowShown="0">
+  <autoFilter ref="J1:Q97" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -9904,14 +9904,14 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Time" dataDxfId="1"/>
-    <tableColumn id="2" name="home_l1"/>
-    <tableColumn id="3" name="home_l2"/>
-    <tableColumn id="4" name="work_l1"/>
-    <tableColumn id="5" name="work_l2"/>
-    <tableColumn id="6" name="public_l2"/>
-    <tableColumn id="7" name="public_l3"/>
-    <tableColumn id="8" name="Total" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Time" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="home_l1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="home_l2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="work_l1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="work_l2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="public_l2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="public_l3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Total" dataDxfId="0">
       <calculatedColumnFormula>SUM(Weekend_EV_Load[[#This Row],[home_l1]:[public_l3]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10215,10 +10215,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -13800,11 +13800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K6" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>